<commit_message>
R script and readme updates
</commit_message>
<xml_diff>
--- a/task.xlsx
+++ b/task.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="45">
   <si>
     <t>speed</t>
   </si>
@@ -160,6 +160,12 @@
     insects are negative
 Go as quickly as you can while being accurate
 Press 'e' or 'i' to continue</t>
+  </si>
+  <si>
+    <t>IRAP_name</t>
+  </si>
+  <si>
+    <t>flowers-insects demo IRAP</t>
   </si>
 </sst>
 </file>
@@ -205,8 +211,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="313">
+  <cellStyleXfs count="315">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -544,7 +552,7 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="313">
+  <cellStyles count="315">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -701,6 +709,7 @@
     <cellStyle name="Followed Hyperlink" xfId="308" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="310" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="312" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="314" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -857,6 +866,7 @@
     <cellStyle name="Hyperlink" xfId="307" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="309" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="311" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="313" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1184,10 +1194,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X4"/>
+  <dimension ref="A1:Y4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -1195,24 +1205,25 @@
     <col min="1" max="1" width="36.140625" style="3" customWidth="1"/>
     <col min="2" max="3" width="37.5703125" style="3" customWidth="1"/>
     <col min="4" max="5" width="15" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="44.42578125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="13.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="26.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17" style="3" customWidth="1"/>
-    <col min="18" max="19" width="14.42578125" style="3" customWidth="1"/>
-    <col min="20" max="21" width="20.7109375" style="3" customWidth="1"/>
-    <col min="22" max="23" width="23.5703125" style="3" customWidth="1"/>
-    <col min="24" max="16384" width="10.7109375" style="3"/>
+    <col min="6" max="6" width="27.28515625" style="3" customWidth="1"/>
+    <col min="7" max="8" width="44.42578125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="26.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17" style="3" customWidth="1"/>
+    <col min="19" max="20" width="14.42578125" style="3" customWidth="1"/>
+    <col min="21" max="22" width="20.7109375" style="3" customWidth="1"/>
+    <col min="23" max="24" width="23.5703125" style="3" customWidth="1"/>
+    <col min="25" max="16384" width="10.7109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:25">
       <c r="A1" s="3" t="s">
         <v>19</v>
       </c>
@@ -1229,64 +1240,67 @@
         <v>13</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="U1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="V1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="W1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="X1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="Y1" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:24" ht="130">
+    <row r="2" spans="1:25" ht="130">
       <c r="A2" s="7" t="s">
         <v>39</v>
       </c>
@@ -1302,71 +1316,76 @@
       <c r="E2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="H2" s="5">
+      <c r="I2" s="5">
         <v>80</v>
       </c>
-      <c r="I2" s="5">
+      <c r="J2" s="5">
         <v>2</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="M2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="N2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="O2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="O2" s="6" t="s">
+      <c r="P2" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="P2" s="3">
+      <c r="Q2" s="3">
         <v>4</v>
       </c>
-      <c r="Q2" s="3">
+      <c r="R2" s="3">
         <v>3</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="S2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="T2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="T2" s="3" t="s">
+      <c r="U2" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="U2" s="3" t="s">
+      <c r="V2" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="V2" s="3" t="s">
+      <c r="W2" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="W2" s="3" t="s">
+      <c r="X2" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="X2" s="3" t="s">
+      <c r="Y2" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:24">
+    <row r="3" spans="1:25">
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="1:24">
+    <row r="4" spans="1:25">
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
quantifies participants who passed practice blocks
</commit_message>
<xml_diff>
--- a/task.xlsx
+++ b/task.xlsx
@@ -1196,8 +1196,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="R3" sqref="R3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
0.9.8 support for multiple sequential IRAPs
</commit_message>
<xml_diff>
--- a/task.xlsx
+++ b/task.xlsx
@@ -162,10 +162,10 @@
 Press 'e' or 'i' to continue</t>
   </si>
   <si>
-    <t>IRAP_name</t>
-  </si>
-  <si>
-    <t>flowers-insects demo IRAP</t>
+    <t>stimulus_file</t>
+  </si>
+  <si>
+    <t>stimuli.xlsx</t>
   </si>
 </sst>
 </file>
@@ -211,8 +211,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="315">
+  <cellStyleXfs count="321">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -552,7 +558,7 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="315">
+  <cellStyles count="321">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -710,6 +716,9 @@
     <cellStyle name="Followed Hyperlink" xfId="310" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="312" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="314" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="316" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="318" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="320" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -867,6 +876,9 @@
     <cellStyle name="Hyperlink" xfId="309" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="311" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="313" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="315" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="317" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="319" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1196,27 +1208,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="R3" sqref="R3"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="36.140625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="18.42578125" style="3" customWidth="1"/>
     <col min="2" max="3" width="37.5703125" style="3" customWidth="1"/>
     <col min="4" max="5" width="15" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.28515625" style="3" customWidth="1"/>
-    <col min="7" max="8" width="44.42578125" style="3" customWidth="1"/>
-    <col min="9" max="9" width="13.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="26.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20" style="3" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="17" style="3" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17" style="3" customWidth="1"/>
+    <col min="11" max="11" width="36.140625" style="3" customWidth="1"/>
+    <col min="12" max="13" width="44.42578125" style="3" customWidth="1"/>
+    <col min="14" max="14" width="6.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="26.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14" style="3" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="19" max="20" width="14.42578125" style="3" customWidth="1"/>
     <col min="21" max="22" width="20.7109375" style="3" customWidth="1"/>
     <col min="23" max="24" width="23.5703125" style="3" customWidth="1"/>
@@ -1225,7 +1237,7 @@
   <sheetData>
     <row r="1" spans="1:25">
       <c r="A1" s="3" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>16</v>
@@ -1240,43 +1252,43 @@
         <v>13</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>43</v>
+        <v>8</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>18</v>
       </c>
       <c r="S1" s="3" t="s">
         <v>22</v>
@@ -1301,8 +1313,8 @@
       </c>
     </row>
     <row r="2" spans="1:25" ht="130">
-      <c r="A2" s="7" t="s">
-        <v>39</v>
+      <c r="A2" s="3" t="s">
+        <v>44</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>42</v>
@@ -1316,44 +1328,44 @@
       <c r="E2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="G2" s="4" t="s">
+      <c r="F2" s="5">
+        <v>80</v>
+      </c>
+      <c r="G2" s="5">
+        <v>2</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" s="3">
+        <v>4</v>
+      </c>
+      <c r="J2" s="3">
+        <v>3</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="L2" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="M2" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="I2" s="5">
-        <v>80</v>
-      </c>
-      <c r="J2" s="5">
+      <c r="N2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="O2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="K2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="M2" s="3" t="s">
+      <c r="P2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="Q2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="R2" s="3" t="s">
         <v>6</v>
-      </c>
-      <c r="P2" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q2" s="3">
-        <v>4</v>
-      </c>
-      <c r="R2" s="3">
-        <v>3</v>
       </c>
       <c r="S2" s="3" t="s">
         <v>30</v>
@@ -1380,12 +1392,10 @@
     <row r="3" spans="1:25">
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
     </row>
     <row r="4" spans="1:25">
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
processing script changes - group by date
</commit_message>
<xml_diff>
--- a/task.xlsx
+++ b/task.xlsx
@@ -1208,8 +1208,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -1329,7 +1329,7 @@
         <v>12</v>
       </c>
       <c r="F2" s="5">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="G2" s="5">
         <v>2</v>
@@ -1341,7 +1341,7 @@
         <v>4</v>
       </c>
       <c r="J2" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K2" s="7" t="s">
         <v>39</v>

</xml_diff>

<commit_message>
update to default stimulus file
</commit_message>
<xml_diff>
--- a/task.xlsx
+++ b/task.xlsx
@@ -1209,7 +1209,7 @@
   <dimension ref="A1:Y4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -1329,7 +1329,7 @@
         <v>12</v>
       </c>
       <c r="F2" s="5">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="G2" s="5">
         <v>2</v>
@@ -1341,7 +1341,7 @@
         <v>4</v>
       </c>
       <c r="J2" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K2" s="7" t="s">
         <v>39</v>

</xml_diff>

<commit_message>
brought D scores in processing script in line with visual basic IRAP versions
Minor change in how RTs were binned; D scores should correlate very
highly (c.99) between both methods, but this way is technically
consistent with previous research. Updates to readme: made images
display properly using relative paths.
</commit_message>
<xml_diff>
--- a/task.xlsx
+++ b/task.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="27226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="27629"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14880" tabRatio="500"/>
@@ -1208,7 +1208,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
@@ -1329,7 +1329,7 @@
         <v>12</v>
       </c>
       <c r="F2" s="5">
-        <v>80</v>
+        <v>0.8</v>
       </c>
       <c r="G2" s="5">
         <v>2</v>

</xml_diff>